<commit_message>
tests tools all work
</commit_message>
<xml_diff>
--- a/defaults/merge.xlsx
+++ b/defaults/merge.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="804">
   <si>
     <t>Index</t>
   </si>
@@ -1438,124 +1438,127 @@
     <t>Sam Hous St</t>
   </si>
   <si>
+    <t>S Alabama</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
+  </si>
+  <si>
+    <t>E Michigan</t>
+  </si>
+  <si>
+    <t>Baylor</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Syracuse</t>
+  </si>
+  <si>
+    <t>Iowa St</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Colorado St</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Fla Atlantic</t>
+  </si>
+  <si>
+    <t>Ball St</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Tulsa</t>
+  </si>
+  <si>
+    <t>GA Tech</t>
+  </si>
+  <si>
+    <t>N Mex State</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Miss State</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Vanderbilt</t>
+  </si>
+  <si>
+    <t>UL Monroe</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Oklahoma St</t>
+  </si>
+  <si>
+    <t>Tulane</t>
+  </si>
+  <si>
+    <t>Notre Dame</t>
+  </si>
+  <si>
+    <t>Fresno St</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Louisville</t>
+  </si>
+  <si>
+    <t>Clemson</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Jksnville St</t>
+  </si>
+  <si>
+    <t>Old Dominion</t>
+  </si>
+  <si>
+    <t>LA Tech</t>
+  </si>
+  <si>
     <t>Alabama</t>
-  </si>
-  <si>
-    <t>Tennessee</t>
-  </si>
-  <si>
-    <t>Texas Tech</t>
-  </si>
-  <si>
-    <t>E Michigan</t>
-  </si>
-  <si>
-    <t>Baylor</t>
-  </si>
-  <si>
-    <t>Miami</t>
-  </si>
-  <si>
-    <t>Syracuse</t>
-  </si>
-  <si>
-    <t>Iowa St</t>
-  </si>
-  <si>
-    <t>Ohio</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Maryland</t>
-  </si>
-  <si>
-    <t>Colorado St</t>
-  </si>
-  <si>
-    <t>Cincinnati</t>
-  </si>
-  <si>
-    <t>New Mexico</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Fla Atlantic</t>
-  </si>
-  <si>
-    <t>Ball St</t>
-  </si>
-  <si>
-    <t>Florida</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>Tulsa</t>
-  </si>
-  <si>
-    <t>GA Tech</t>
-  </si>
-  <si>
-    <t>N Mex State</t>
-  </si>
-  <si>
-    <t>Oklahoma</t>
-  </si>
-  <si>
-    <t>Miss State</t>
-  </si>
-  <si>
-    <t>Missouri</t>
-  </si>
-  <si>
-    <t>Vanderbilt</t>
-  </si>
-  <si>
-    <t>UL Monroe</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Oklahoma St</t>
-  </si>
-  <si>
-    <t>Tulane</t>
-  </si>
-  <si>
-    <t>Notre Dame</t>
-  </si>
-  <si>
-    <t>Fresno St</t>
-  </si>
-  <si>
-    <t>Nevada</t>
-  </si>
-  <si>
-    <t>Louisville</t>
-  </si>
-  <si>
-    <t>Clemson</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Jksnville St</t>
-  </si>
-  <si>
-    <t>Old Dominion</t>
-  </si>
-  <si>
-    <t>LA Tech</t>
   </si>
   <si>
     <t>Air Force</t>
@@ -2817,7 +2820,7 @@
         <v>461</v>
       </c>
       <c r="E2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2834,7 +2837,7 @@
         <v>462</v>
       </c>
       <c r="E3" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2851,7 +2854,7 @@
         <v>463</v>
       </c>
       <c r="E4" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2868,7 +2871,7 @@
         <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2885,7 +2888,7 @@
         <v>465</v>
       </c>
       <c r="E6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2902,7 +2905,7 @@
         <v>465</v>
       </c>
       <c r="E7" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2919,7 +2922,7 @@
         <v>465</v>
       </c>
       <c r="E8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2936,7 +2939,7 @@
         <v>466</v>
       </c>
       <c r="E9" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2953,7 +2956,7 @@
         <v>467</v>
       </c>
       <c r="E10" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2970,7 +2973,7 @@
         <v>468</v>
       </c>
       <c r="E11" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2987,7 +2990,7 @@
         <v>465</v>
       </c>
       <c r="E12" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3004,7 +3007,7 @@
         <v>465</v>
       </c>
       <c r="E13" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3021,7 +3024,7 @@
         <v>465</v>
       </c>
       <c r="E14" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3038,7 +3041,7 @@
         <v>469</v>
       </c>
       <c r="E15" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3055,7 +3058,7 @@
         <v>470</v>
       </c>
       <c r="E16" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3072,7 +3075,7 @@
         <v>471</v>
       </c>
       <c r="E17" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3089,7 +3092,7 @@
         <v>472</v>
       </c>
       <c r="E18" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3106,7 +3109,7 @@
         <v>473</v>
       </c>
       <c r="E19" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3123,7 +3126,7 @@
         <v>465</v>
       </c>
       <c r="E20" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3140,7 +3143,7 @@
         <v>465</v>
       </c>
       <c r="E21" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3157,7 +3160,7 @@
         <v>465</v>
       </c>
       <c r="E22" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3174,7 +3177,7 @@
         <v>465</v>
       </c>
       <c r="E23" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3191,7 +3194,7 @@
         <v>465</v>
       </c>
       <c r="E24" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3208,7 +3211,7 @@
         <v>465</v>
       </c>
       <c r="E25" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3225,7 +3228,7 @@
         <v>465</v>
       </c>
       <c r="E26" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3242,7 +3245,7 @@
         <v>474</v>
       </c>
       <c r="E27" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3259,7 +3262,7 @@
         <v>465</v>
       </c>
       <c r="E28" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3276,7 +3279,7 @@
         <v>465</v>
       </c>
       <c r="E29" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3293,7 +3296,7 @@
         <v>475</v>
       </c>
       <c r="E30" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3310,7 +3313,7 @@
         <v>476</v>
       </c>
       <c r="E31" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3327,7 +3330,7 @@
         <v>465</v>
       </c>
       <c r="E32" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3344,7 +3347,7 @@
         <v>264</v>
       </c>
       <c r="E33" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3361,7 +3364,7 @@
         <v>465</v>
       </c>
       <c r="E34" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3378,7 +3381,7 @@
         <v>465</v>
       </c>
       <c r="E35" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3395,7 +3398,7 @@
         <v>477</v>
       </c>
       <c r="E36" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -3412,7 +3415,7 @@
         <v>478</v>
       </c>
       <c r="E37" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3429,7 +3432,7 @@
         <v>479</v>
       </c>
       <c r="E38" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3446,7 +3449,7 @@
         <v>270</v>
       </c>
       <c r="E39" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3463,7 +3466,7 @@
         <v>480</v>
       </c>
       <c r="E40" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3480,7 +3483,7 @@
         <v>481</v>
       </c>
       <c r="E41" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3497,7 +3500,7 @@
         <v>465</v>
       </c>
       <c r="E42" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3514,7 +3517,7 @@
         <v>482</v>
       </c>
       <c r="E43" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3531,7 +3534,7 @@
         <v>465</v>
       </c>
       <c r="E44" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3548,7 +3551,7 @@
         <v>483</v>
       </c>
       <c r="E45" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3565,7 +3568,7 @@
         <v>465</v>
       </c>
       <c r="E46" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3582,7 +3585,7 @@
         <v>484</v>
       </c>
       <c r="E47" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3599,7 +3602,7 @@
         <v>485</v>
       </c>
       <c r="E48" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3616,7 +3619,7 @@
         <v>465</v>
       </c>
       <c r="E49" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3633,7 +3636,7 @@
         <v>486</v>
       </c>
       <c r="E50" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -3650,7 +3653,7 @@
         <v>487</v>
       </c>
       <c r="E51" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -3684,7 +3687,7 @@
         <v>489</v>
       </c>
       <c r="E53" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3701,7 +3704,7 @@
         <v>490</v>
       </c>
       <c r="E54" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3718,7 +3721,7 @@
         <v>491</v>
       </c>
       <c r="E55" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3735,7 +3738,7 @@
         <v>492</v>
       </c>
       <c r="E56" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3752,7 +3755,7 @@
         <v>493</v>
       </c>
       <c r="E57" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3769,7 +3772,7 @@
         <v>465</v>
       </c>
       <c r="E58" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3786,7 +3789,7 @@
         <v>465</v>
       </c>
       <c r="E59" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3803,7 +3806,7 @@
         <v>494</v>
       </c>
       <c r="E60" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3820,7 +3823,7 @@
         <v>495</v>
       </c>
       <c r="E61" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3837,7 +3840,7 @@
         <v>465</v>
       </c>
       <c r="E62" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3854,7 +3857,7 @@
         <v>465</v>
       </c>
       <c r="E63" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3871,7 +3874,7 @@
         <v>496</v>
       </c>
       <c r="E64" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3888,7 +3891,7 @@
         <v>465</v>
       </c>
       <c r="E65" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3905,7 +3908,7 @@
         <v>497</v>
       </c>
       <c r="E66" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3922,7 +3925,7 @@
         <v>498</v>
       </c>
       <c r="E67" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3939,7 +3942,7 @@
         <v>465</v>
       </c>
       <c r="E68" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3956,7 +3959,7 @@
         <v>499</v>
       </c>
       <c r="E69" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3973,7 +3976,7 @@
         <v>500</v>
       </c>
       <c r="E70" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3990,7 +3993,7 @@
         <v>501</v>
       </c>
       <c r="E71" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4024,7 +4027,7 @@
         <v>503</v>
       </c>
       <c r="E73" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -4041,7 +4044,7 @@
         <v>504</v>
       </c>
       <c r="E74" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4058,7 +4061,7 @@
         <v>465</v>
       </c>
       <c r="E75" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -4075,7 +4078,7 @@
         <v>307</v>
       </c>
       <c r="E76" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4092,7 +4095,7 @@
         <v>465</v>
       </c>
       <c r="E77" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4109,7 +4112,7 @@
         <v>505</v>
       </c>
       <c r="E78" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4126,7 +4129,7 @@
         <v>465</v>
       </c>
       <c r="E79" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -4143,7 +4146,7 @@
         <v>465</v>
       </c>
       <c r="E80" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -4160,7 +4163,7 @@
         <v>465</v>
       </c>
       <c r="E81" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -4177,7 +4180,7 @@
         <v>506</v>
       </c>
       <c r="E82" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -4194,7 +4197,7 @@
         <v>465</v>
       </c>
       <c r="E83" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -4211,7 +4214,7 @@
         <v>465</v>
       </c>
       <c r="E84" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -4228,7 +4231,7 @@
         <v>465</v>
       </c>
       <c r="E85" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -4245,7 +4248,7 @@
         <v>507</v>
       </c>
       <c r="E86" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -4262,7 +4265,7 @@
         <v>508</v>
       </c>
       <c r="E87" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4279,7 +4282,7 @@
         <v>509</v>
       </c>
       <c r="E88" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4296,7 +4299,7 @@
         <v>510</v>
       </c>
       <c r="E89" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -4313,7 +4316,7 @@
         <v>511</v>
       </c>
       <c r="E90" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -4330,7 +4333,7 @@
         <v>512</v>
       </c>
       <c r="E91" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -4347,7 +4350,7 @@
         <v>513</v>
       </c>
       <c r="E92" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -4381,7 +4384,7 @@
         <v>465</v>
       </c>
       <c r="E94" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -4398,7 +4401,7 @@
         <v>326</v>
       </c>
       <c r="E95" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -4415,7 +4418,7 @@
         <v>465</v>
       </c>
       <c r="E96" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -4429,10 +4432,10 @@
         <v>328</v>
       </c>
       <c r="D97" t="s">
-        <v>474</v>
+        <v>514</v>
       </c>
       <c r="E97" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4446,10 +4449,10 @@
         <v>329</v>
       </c>
       <c r="D98" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E98" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4466,7 +4469,7 @@
         <v>465</v>
       </c>
       <c r="E99" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -4483,7 +4486,7 @@
         <v>465</v>
       </c>
       <c r="E100" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -4500,7 +4503,7 @@
         <v>465</v>
       </c>
       <c r="E101" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -4514,10 +4517,10 @@
         <v>333</v>
       </c>
       <c r="D102" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E102" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4534,7 +4537,7 @@
         <v>498</v>
       </c>
       <c r="E103" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -4548,10 +4551,10 @@
         <v>335</v>
       </c>
       <c r="D104" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="E104" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4565,10 +4568,10 @@
         <v>336</v>
       </c>
       <c r="D105" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E105" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -4585,7 +4588,7 @@
         <v>465</v>
       </c>
       <c r="E106" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -4602,7 +4605,7 @@
         <v>338</v>
       </c>
       <c r="E107" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -4619,7 +4622,7 @@
         <v>465</v>
       </c>
       <c r="E108" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4636,7 +4639,7 @@
         <v>465</v>
       </c>
       <c r="E109" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -4650,10 +4653,10 @@
         <v>341</v>
       </c>
       <c r="D110" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E110" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -4684,10 +4687,10 @@
         <v>343</v>
       </c>
       <c r="D112" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="E112" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -4701,10 +4704,10 @@
         <v>344</v>
       </c>
       <c r="D113" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E113" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -4718,10 +4721,10 @@
         <v>345</v>
       </c>
       <c r="D114" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="E114" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -4735,10 +4738,10 @@
         <v>346</v>
       </c>
       <c r="D115" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E115" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -4752,10 +4755,10 @@
         <v>347</v>
       </c>
       <c r="D116" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E116" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4772,7 +4775,7 @@
         <v>465</v>
       </c>
       <c r="E117" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4786,10 +4789,10 @@
         <v>349</v>
       </c>
       <c r="D118" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="E118" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -4803,10 +4806,10 @@
         <v>350</v>
       </c>
       <c r="D119" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E119" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -4823,7 +4826,7 @@
         <v>351</v>
       </c>
       <c r="E120" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -4837,10 +4840,10 @@
         <v>352</v>
       </c>
       <c r="D121" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E121" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -4857,7 +4860,7 @@
         <v>513</v>
       </c>
       <c r="E122" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -4871,10 +4874,10 @@
         <v>354</v>
       </c>
       <c r="D123" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E123" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4891,7 +4894,7 @@
         <v>465</v>
       </c>
       <c r="E124" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4908,7 +4911,7 @@
         <v>465</v>
       </c>
       <c r="E125" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -4922,10 +4925,10 @@
         <v>357</v>
       </c>
       <c r="D126" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="E126" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -4942,7 +4945,7 @@
         <v>465</v>
       </c>
       <c r="E127" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -4959,7 +4962,7 @@
         <v>465</v>
       </c>
       <c r="E128" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4976,7 +4979,7 @@
         <v>465</v>
       </c>
       <c r="E129" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4990,10 +4993,10 @@
         <v>361</v>
       </c>
       <c r="D130" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="E130" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -5007,10 +5010,10 @@
         <v>362</v>
       </c>
       <c r="D131" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E131" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -5024,10 +5027,10 @@
         <v>363</v>
       </c>
       <c r="D132" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E132" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -5044,7 +5047,7 @@
         <v>465</v>
       </c>
       <c r="E133" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -5058,10 +5061,10 @@
         <v>365</v>
       </c>
       <c r="D134" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E134" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -5075,10 +5078,10 @@
         <v>366</v>
       </c>
       <c r="D135" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E135" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -5092,10 +5095,10 @@
         <v>367</v>
       </c>
       <c r="D136" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E136" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -5109,10 +5112,10 @@
         <v>368</v>
       </c>
       <c r="D137" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E137" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -5126,10 +5129,10 @@
         <v>369</v>
       </c>
       <c r="D138" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E138" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -5146,7 +5149,7 @@
         <v>465</v>
       </c>
       <c r="E139" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -5163,7 +5166,7 @@
         <v>465</v>
       </c>
       <c r="E140" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -5180,7 +5183,7 @@
         <v>465</v>
       </c>
       <c r="E141" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -5197,7 +5200,7 @@
         <v>465</v>
       </c>
       <c r="E142" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -5214,7 +5217,7 @@
         <v>465</v>
       </c>
       <c r="E143" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -5231,7 +5234,7 @@
         <v>465</v>
       </c>
       <c r="E144" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -5245,10 +5248,10 @@
         <v>376</v>
       </c>
       <c r="D145" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="E145" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -5262,7 +5265,7 @@
         <v>377</v>
       </c>
       <c r="D146" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E146" t="s">
         <v>377</v>
@@ -5279,10 +5282,10 @@
         <v>378</v>
       </c>
       <c r="D147" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E147" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -5299,7 +5302,7 @@
         <v>465</v>
       </c>
       <c r="E148" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5316,7 +5319,7 @@
         <v>465</v>
       </c>
       <c r="E149" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5330,10 +5333,10 @@
         <v>381</v>
       </c>
       <c r="D150" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E150" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5350,7 +5353,7 @@
         <v>465</v>
       </c>
       <c r="E151" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5364,10 +5367,10 @@
         <v>383</v>
       </c>
       <c r="D152" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E152" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5381,10 +5384,10 @@
         <v>384</v>
       </c>
       <c r="D153" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="E153" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5398,10 +5401,10 @@
         <v>385</v>
       </c>
       <c r="D154" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E154" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5418,7 +5421,7 @@
         <v>465</v>
       </c>
       <c r="E155" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5432,10 +5435,10 @@
         <v>387</v>
       </c>
       <c r="D156" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E156" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5452,7 +5455,7 @@
         <v>388</v>
       </c>
       <c r="E157" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5466,10 +5469,10 @@
         <v>389</v>
       </c>
       <c r="D158" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="E158" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5483,10 +5486,10 @@
         <v>390</v>
       </c>
       <c r="D159" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E159" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5500,7 +5503,7 @@
         <v>391</v>
       </c>
       <c r="D160" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E160" t="s">
         <v>391</v>
@@ -5517,10 +5520,10 @@
         <v>392</v>
       </c>
       <c r="D161" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E161" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -5534,10 +5537,10 @@
         <v>393</v>
       </c>
       <c r="D162" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E162" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -5554,7 +5557,7 @@
         <v>465</v>
       </c>
       <c r="E163" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -5568,10 +5571,10 @@
         <v>395</v>
       </c>
       <c r="D164" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E164" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5585,10 +5588,10 @@
         <v>396</v>
       </c>
       <c r="D165" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E165" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5605,7 +5608,7 @@
         <v>465</v>
       </c>
       <c r="E166" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -5619,10 +5622,10 @@
         <v>398</v>
       </c>
       <c r="D167" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E167" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -5636,10 +5639,10 @@
         <v>399</v>
       </c>
       <c r="D168" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="E168" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -5656,7 +5659,7 @@
         <v>465</v>
       </c>
       <c r="E169" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -5670,10 +5673,10 @@
         <v>401</v>
       </c>
       <c r="D170" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E170" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -5687,10 +5690,10 @@
         <v>402</v>
       </c>
       <c r="D171" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E171" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -5707,7 +5710,7 @@
         <v>510</v>
       </c>
       <c r="E172" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -5721,10 +5724,10 @@
         <v>404</v>
       </c>
       <c r="D173" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="E173" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -5738,10 +5741,10 @@
         <v>405</v>
       </c>
       <c r="D174" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E174" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -5758,7 +5761,7 @@
         <v>465</v>
       </c>
       <c r="E175" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -5775,7 +5778,7 @@
         <v>465</v>
       </c>
       <c r="E176" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5792,7 +5795,7 @@
         <v>465</v>
       </c>
       <c r="E177" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="178" spans="1:5">
@@ -5809,7 +5812,7 @@
         <v>465</v>
       </c>
       <c r="E178" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -5823,10 +5826,10 @@
         <v>410</v>
       </c>
       <c r="D179" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E179" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -5840,10 +5843,10 @@
         <v>411</v>
       </c>
       <c r="D180" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E180" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -5857,10 +5860,10 @@
         <v>412</v>
       </c>
       <c r="D181" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E181" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -5874,10 +5877,10 @@
         <v>413</v>
       </c>
       <c r="D182" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E182" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5894,7 +5897,7 @@
         <v>465</v>
       </c>
       <c r="E183" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -5911,7 +5914,7 @@
         <v>465</v>
       </c>
       <c r="E184" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5928,7 +5931,7 @@
         <v>465</v>
       </c>
       <c r="E185" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -5945,7 +5948,7 @@
         <v>465</v>
       </c>
       <c r="E186" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5959,10 +5962,10 @@
         <v>418</v>
       </c>
       <c r="D187" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E187" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5979,7 +5982,7 @@
         <v>465</v>
       </c>
       <c r="E188" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5996,7 +5999,7 @@
         <v>492</v>
       </c>
       <c r="E189" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -6013,7 +6016,7 @@
         <v>465</v>
       </c>
       <c r="E190" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -6027,10 +6030,10 @@
         <v>422</v>
       </c>
       <c r="D191" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E191" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -6047,7 +6050,7 @@
         <v>499</v>
       </c>
       <c r="E192" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -6061,10 +6064,10 @@
         <v>424</v>
       </c>
       <c r="D193" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="E193" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -6078,10 +6081,10 @@
         <v>425</v>
       </c>
       <c r="D194" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E194" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -6095,10 +6098,10 @@
         <v>426</v>
       </c>
       <c r="D195" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E195" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -6112,10 +6115,10 @@
         <v>427</v>
       </c>
       <c r="D196" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E196" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -6129,10 +6132,10 @@
         <v>428</v>
       </c>
       <c r="D197" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="E197" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -6146,10 +6149,10 @@
         <v>429</v>
       </c>
       <c r="D198" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E198" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -6166,7 +6169,7 @@
         <v>465</v>
       </c>
       <c r="E199" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -6183,7 +6186,7 @@
         <v>465</v>
       </c>
       <c r="E200" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -6197,7 +6200,7 @@
         <v>432</v>
       </c>
       <c r="D201" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E201" t="s">
         <v>432</v>
@@ -6214,10 +6217,10 @@
         <v>433</v>
       </c>
       <c r="D202" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="E202" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -6231,10 +6234,10 @@
         <v>434</v>
       </c>
       <c r="D203" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="E203" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -6248,10 +6251,10 @@
         <v>435</v>
       </c>
       <c r="D204" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="E204" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -6265,10 +6268,10 @@
         <v>436</v>
       </c>
       <c r="D205" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E205" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -6285,7 +6288,7 @@
         <v>465</v>
       </c>
       <c r="E206" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -6299,10 +6302,10 @@
         <v>438</v>
       </c>
       <c r="D207" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E207" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -6316,10 +6319,10 @@
         <v>439</v>
       </c>
       <c r="D208" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E208" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -6333,10 +6336,10 @@
         <v>440</v>
       </c>
       <c r="D209" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E209" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -6350,10 +6353,10 @@
         <v>441</v>
       </c>
       <c r="D210" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="E210" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -6370,7 +6373,7 @@
         <v>465</v>
       </c>
       <c r="E211" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -6384,10 +6387,10 @@
         <v>443</v>
       </c>
       <c r="D212" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="E212" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -6404,7 +6407,7 @@
         <v>465</v>
       </c>
       <c r="E213" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -6418,7 +6421,7 @@
         <v>445</v>
       </c>
       <c r="D214" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="E214" t="s">
         <v>445</v>
@@ -6438,7 +6441,7 @@
         <v>465</v>
       </c>
       <c r="E215" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -6452,10 +6455,10 @@
         <v>447</v>
       </c>
       <c r="D216" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="E216" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -6472,7 +6475,7 @@
         <v>448</v>
       </c>
       <c r="E217" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6489,7 +6492,7 @@
         <v>463</v>
       </c>
       <c r="E218" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -6503,10 +6506,10 @@
         <v>450</v>
       </c>
       <c r="D219" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="E219" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -6520,10 +6523,10 @@
         <v>451</v>
       </c>
       <c r="D220" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E220" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -6537,10 +6540,10 @@
         <v>452</v>
       </c>
       <c r="D221" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E221" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6557,7 +6560,7 @@
         <v>465</v>
       </c>
       <c r="E222" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6574,7 +6577,7 @@
         <v>465</v>
       </c>
       <c r="E223" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -6588,10 +6591,10 @@
         <v>455</v>
       </c>
       <c r="D224" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E224" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6605,10 +6608,10 @@
         <v>456</v>
       </c>
       <c r="D225" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E225" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6625,7 +6628,7 @@
         <v>465</v>
       </c>
       <c r="E226" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6639,10 +6642,10 @@
         <v>458</v>
       </c>
       <c r="D227" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E227" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6656,10 +6659,10 @@
         <v>459</v>
       </c>
       <c r="D228" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="E228" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6673,10 +6676,10 @@
         <v>460</v>
       </c>
       <c r="D229" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="E229" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>

</xml_diff>